<commit_message>
figuras sombreadas y dataset
</commit_message>
<xml_diff>
--- a/data/raw/tabulada/pozos_seleccion.xlsx
+++ b/data/raw/tabulada/pozos_seleccion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hemera\acongagua\data\raw\tabulada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7286E20-13DF-4619-8672-DFAC093D008F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31883B73-EB4A-4F08-9555-DD43790BA58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="735" windowWidth="16200" windowHeight="8295" xr2:uid="{1B23D121-3738-4D5E-BC26-2F0986B747F3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{1B23D121-3738-4D5E-BC26-2F0986B747F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,20 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>SHAC_216</t>
-  </si>
-  <si>
-    <t>SHAC_217</t>
-  </si>
-  <si>
-    <t>SHAC_220</t>
-  </si>
-  <si>
-    <t>SHAC_221</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,23 +415,23 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="A1">
+        <v>216</v>
+      </c>
+      <c r="B1">
+        <v>217</v>
+      </c>
+      <c r="C1">
+        <v>220</v>
+      </c>
+      <c r="D1">
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>